<commit_message>
Actualización TASK, SCHEDULE hasta semana 7
</commit_message>
<xml_diff>
--- a/NoteBook/task and schedule plans and actual/TASK_Fabian Becerra_Ciclo2.xlsx
+++ b/NoteBook/task and schedule plans and actual/TASK_Fabian Becerra_Ciclo2.xlsx
@@ -432,6 +432,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -450,6 +484,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -459,55 +508,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,12 +835,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -849,202 +849,202 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="34">
         <v>41748</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="30">
         <v>2</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="12" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="12" t="s">
+      <c r="E7" s="26"/>
+      <c r="F7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12" t="s">
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="26"/>
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="27" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
     </row>
     <row r="13" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="12">
         <v>0.3</v>
       </c>
       <c r="E14" s="8">
@@ -1079,14 +1079,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="12">
         <v>0.3</v>
       </c>
       <c r="E15" s="7">
@@ -1122,12 +1122,12 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="12">
         <v>1</v>
       </c>
       <c r="E16" s="7">
@@ -1163,14 +1163,14 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="12">
         <v>0.2</v>
       </c>
       <c r="E17" s="7">
@@ -1206,12 +1206,12 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="12">
         <v>0.5</v>
       </c>
       <c r="E18" s="7">
@@ -1247,12 +1247,12 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="12">
         <v>1</v>
       </c>
       <c r="E19" s="7">
@@ -1288,12 +1288,12 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="12">
         <v>1</v>
       </c>
       <c r="E20" s="7">
@@ -1329,14 +1329,14 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="13">
         <v>1</v>
       </c>
       <c r="E21" s="7">
@@ -1356,20 +1356,24 @@
         <f t="shared" si="1"/>
         <v>18.399999999999999</v>
       </c>
-      <c r="K21" s="10"/>
+      <c r="K21" s="10">
+        <v>1</v>
+      </c>
       <c r="L21" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
-      </c>
-      <c r="M21" s="10"/>
+        <v>6.12</v>
+      </c>
+      <c r="M21" s="10">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="13">
         <v>2</v>
       </c>
       <c r="E22" s="7">
@@ -1393,22 +1397,26 @@
         <f t="shared" si="1"/>
         <v>25.299999999999997</v>
       </c>
-      <c r="K22" s="10"/>
+      <c r="K22" s="10">
+        <v>2.5</v>
+      </c>
       <c r="L22" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
-      </c>
-      <c r="M22" s="10"/>
+        <v>8.620000000000001</v>
+      </c>
+      <c r="M22" s="10">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="14">
         <v>1</v>
       </c>
       <c r="E23" s="7">
@@ -1435,17 +1443,17 @@
       <c r="K23" s="10"/>
       <c r="L23" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M23" s="10"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="14">
         <v>2</v>
       </c>
       <c r="E24" s="7">
@@ -1472,17 +1480,17 @@
       <c r="K24" s="10"/>
       <c r="L24" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="14">
         <v>3</v>
       </c>
       <c r="E25" s="7">
@@ -1509,17 +1517,17 @@
       <c r="K25" s="10"/>
       <c r="L25" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M25" s="10"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="14">
         <v>2</v>
       </c>
       <c r="E26" s="7">
@@ -1546,19 +1554,19 @@
       <c r="K26" s="10"/>
       <c r="L26" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M26" s="10"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="14">
         <v>1</v>
       </c>
       <c r="E27" s="7">
@@ -1585,17 +1593,17 @@
       <c r="K27" s="10"/>
       <c r="L27" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="31">
+      <c r="D28" s="14">
         <v>1.5</v>
       </c>
       <c r="E28" s="7">
@@ -1622,17 +1630,17 @@
       <c r="K28" s="10"/>
       <c r="L28" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M28" s="10"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="14">
         <v>1</v>
       </c>
       <c r="E29" s="7">
@@ -1659,17 +1667,17 @@
       <c r="K29" s="10"/>
       <c r="L29" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M29" s="10"/>
     </row>
     <row r="30" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="23"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="14">
         <v>2</v>
       </c>
       <c r="E30" s="7">
@@ -1696,17 +1704,17 @@
       <c r="K30" s="10"/>
       <c r="L30" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M30" s="10"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="28"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="31">
+      <c r="D31" s="14">
         <v>1</v>
       </c>
       <c r="E31" s="7">
@@ -1733,19 +1741,19 @@
       <c r="K31" s="10"/>
       <c r="L31" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M31" s="10"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="5"/>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="15">
         <v>0.5</v>
       </c>
       <c r="E32" s="7">
@@ -1772,17 +1780,17 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M32" s="7"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="23"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="15">
         <v>0.5</v>
       </c>
       <c r="E33" s="7">
@@ -1809,17 +1817,17 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M33" s="7"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="23"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="32">
+      <c r="D34" s="15">
         <v>1</v>
       </c>
       <c r="E34" s="7">
@@ -1846,17 +1854,17 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M34" s="7"/>
     </row>
     <row r="35" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="9"/>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="32">
+      <c r="D35" s="15">
         <v>2</v>
       </c>
       <c r="E35" s="7">
@@ -1883,17 +1891,17 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M35" s="7"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="23"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="32">
+      <c r="D36" s="15">
         <v>1</v>
       </c>
       <c r="E36" s="7">
@@ -1920,17 +1928,17 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="9"/>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="32">
+      <c r="D37" s="15">
         <v>1</v>
       </c>
       <c r="E37" s="7">
@@ -1957,17 +1965,17 @@
       <c r="K37" s="7"/>
       <c r="L37" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M37" s="7"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="9"/>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="32">
+      <c r="D38" s="15">
         <v>1</v>
       </c>
       <c r="E38" s="7">
@@ -1990,7 +1998,7 @@
       <c r="K38" s="7"/>
       <c r="L38" s="7">
         <f t="shared" si="2"/>
-        <v>5.12</v>
+        <v>8.620000000000001</v>
       </c>
       <c r="M38" s="7"/>
     </row>
@@ -1999,13 +2007,32 @@
         <f>SUM(D14:D38)</f>
         <v>28.8</v>
       </c>
-      <c r="I39" s="37">
+      <c r="I39" s="20">
         <f>SUM(I14:I38)</f>
         <v>99.9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="K8:K13"/>
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="M8:M13"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E3:G3"/>
     <mergeCell ref="A32:A38"/>
     <mergeCell ref="F7:J7"/>
     <mergeCell ref="J8:J13"/>
@@ -2017,25 +2044,6 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A27:A31"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="D8:D13"/>
-    <mergeCell ref="K8:K13"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="M8:M13"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="G8:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización WEEK personal semana 7
</commit_message>
<xml_diff>
--- a/NoteBook/task and schedule plans and actual/TASK_Fabian Becerra_Ciclo2.xlsx
+++ b/NoteBook/task and schedule plans and actual/TASK_Fabian Becerra_Ciclo2.xlsx
@@ -457,36 +457,42 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -499,13 +505,7 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,12 +835,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -849,18 +849,18 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="34">
+      <c r="E3" s="36">
         <v>41748</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -883,8 +883,8 @@
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
@@ -898,143 +898,143 @@
       <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="24" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="24" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="24" t="s">
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="26"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="23"/>
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="27" t="s">
+      <c r="M8" s="24" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
@@ -1079,7 +1079,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="31" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="5"/>
@@ -1122,7 +1122,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="5"/>
       <c r="C16" s="16" t="s">
         <v>25</v>
@@ -1163,7 +1163,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="5"/>
@@ -1206,7 +1206,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5"/>
       <c r="C18" s="16" t="s">
         <v>31</v>
@@ -1247,7 +1247,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="5"/>
       <c r="C19" s="16" t="s">
         <v>42</v>
@@ -1288,7 +1288,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="5"/>
       <c r="C20" s="16" t="s">
         <v>43</v>
@@ -1329,7 +1329,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="31" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="5"/>
@@ -1368,7 +1368,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="5"/>
       <c r="C22" s="17" t="s">
         <v>45</v>
@@ -1409,7 +1409,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="31" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="5"/>
@@ -1448,7 +1448,7 @@
       <c r="M23" s="10"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="5"/>
       <c r="C24" s="18" t="s">
         <v>47</v>
@@ -1485,7 +1485,7 @@
       <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="5"/>
       <c r="C25" s="18" t="s">
         <v>26</v>
@@ -1522,7 +1522,7 @@
       <c r="M25" s="10"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="5"/>
       <c r="C26" s="18" t="s">
         <v>48</v>
@@ -1559,7 +1559,7 @@
       <c r="M26" s="10"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B27" s="5"/>
@@ -1598,7 +1598,7 @@
       <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="5"/>
       <c r="C28" s="18" t="s">
         <v>50</v>
@@ -1635,7 +1635,7 @@
       <c r="M28" s="10"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="5"/>
       <c r="C29" s="18" t="s">
         <v>51</v>
@@ -1672,7 +1672,7 @@
       <c r="M29" s="10"/>
     </row>
     <row r="30" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="5"/>
       <c r="C30" s="18" t="s">
         <v>45</v>
@@ -1709,7 +1709,7 @@
       <c r="M30" s="10"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="23"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="5"/>
       <c r="C31" s="18" t="s">
         <v>52</v>
@@ -1746,7 +1746,7 @@
       <c r="M31" s="10"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="31" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="5"/>
@@ -1785,7 +1785,7 @@
       <c r="M32" s="7"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="9"/>
       <c r="C33" s="19" t="s">
         <v>54</v>
@@ -1822,7 +1822,7 @@
       <c r="M33" s="7"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="9"/>
       <c r="C34" s="19" t="s">
         <v>27</v>
@@ -1859,7 +1859,7 @@
       <c r="M34" s="7"/>
     </row>
     <row r="35" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="22"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="9"/>
       <c r="C35" s="19" t="s">
         <v>45</v>
@@ -1896,7 +1896,7 @@
       <c r="M35" s="7"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="22"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="9"/>
       <c r="C36" s="19" t="s">
         <v>52</v>
@@ -1933,7 +1933,7 @@
       <c r="M36" s="7"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="22"/>
+      <c r="A37" s="32"/>
       <c r="B37" s="9"/>
       <c r="C37" s="19" t="s">
         <v>55</v>
@@ -1970,7 +1970,7 @@
       <c r="M37" s="7"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="23"/>
+      <c r="A38" s="37"/>
       <c r="B38" s="9"/>
       <c r="C38" s="19" t="s">
         <v>56</v>
@@ -2014,25 +2014,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="D8:D13"/>
-    <mergeCell ref="K8:K13"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="M8:M13"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E3:G3"/>
     <mergeCell ref="A32:A38"/>
     <mergeCell ref="F7:J7"/>
     <mergeCell ref="J8:J13"/>
@@ -2044,6 +2025,25 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A27:A31"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="K8:K13"/>
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="M8:M13"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="G8:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>